<commit_message>
general updates, working on CPAP effector beta files
</commit_message>
<xml_diff>
--- a/Teeny Weeny BOM.xlsx
+++ b/Teeny Weeny BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\26-1_fea\Documents\Reilly_Projects\Teeny Weeny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E27D29-EAF8-4A6A-844F-5C3A999DB959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6315DC42-5151-4CB4-A4CC-446B47C1CE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Amazon</t>
   </si>
@@ -307,6 +307,18 @@
   </si>
   <si>
     <t>M2.5 standoffs and fasteners for electornics and effector</t>
+  </si>
+  <si>
+    <t>High Speed Turbine Fan with Nidec Brushless Motor and Built-in Drive for Sweeper and Vacuum Cleaner - AliExpress 1420</t>
+  </si>
+  <si>
+    <t>CPAP Driver Board (IF using CPAP toolhead)</t>
+  </si>
+  <si>
+    <t>Roborock Blower Fan</t>
+  </si>
+  <si>
+    <t>Ldee5bgs173tw01|roborock S50 S51 S52 S55 Motor Replacement - Xiaomi Mi Robot Sdjqr01rr Parts (aliexpress.us)</t>
   </si>
 </sst>
 </file>
@@ -710,10 +722,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1021"/>
+  <dimension ref="A1:Z1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2323,74 +2335,72 @@
       <c r="Z51" s="8"/>
     </row>
     <row r="52" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="4"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
-      <c r="N52" s="4"/>
-      <c r="O52" s="4"/>
-      <c r="P52" s="4"/>
-      <c r="Q52" s="4"/>
-      <c r="R52" s="4"/>
-      <c r="S52" s="4"/>
-      <c r="T52" s="4"/>
-      <c r="U52" s="4"/>
-      <c r="V52" s="4"/>
-      <c r="W52" s="4"/>
-      <c r="X52" s="4"/>
-      <c r="Y52" s="4"/>
-      <c r="Z52" s="4"/>
+      <c r="A52" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="8"/>
+      <c r="R52" s="8"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8"/>
+      <c r="U52" s="8"/>
+      <c r="V52" s="8"/>
+      <c r="W52" s="8"/>
+      <c r="X52" s="8"/>
+      <c r="Y52" s="8"/>
+      <c r="Z52" s="8"/>
     </row>
     <row r="53" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="22" t="s">
-        <v>25</v>
+      <c r="A53" s="8" t="s">
+        <v>86</v>
       </c>
-      <c r="B53" s="23">
-        <f>SUM(B3:B49)</f>
-        <v>113.18</v>
+      <c r="B53" s="9"/>
+      <c r="C53" s="26" t="s">
+        <v>87</v>
       </c>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
-      <c r="P53" s="4"/>
-      <c r="Q53" s="4"/>
-      <c r="R53" s="4"/>
-      <c r="S53" s="4"/>
-      <c r="T53" s="4"/>
-      <c r="U53" s="4"/>
-      <c r="V53" s="4"/>
-      <c r="W53" s="4"/>
-      <c r="X53" s="4"/>
-      <c r="Y53" s="4"/>
-      <c r="Z53" s="4"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="8"/>
+      <c r="Q53" s="8"/>
+      <c r="R53" s="8"/>
+      <c r="S53" s="8"/>
+      <c r="T53" s="8"/>
+      <c r="U53" s="8"/>
+      <c r="V53" s="8"/>
+      <c r="W53" s="8"/>
+      <c r="X53" s="8"/>
+      <c r="Y53" s="8"/>
+      <c r="Z53" s="8"/>
     </row>
     <row r="54" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B54" s="23" t="e">
-        <f ca="1">MULTIPLY(B53,0.78)</f>
-        <v>#NAME?</v>
-      </c>
+      <c r="A54" s="4"/>
+      <c r="B54" s="7"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -2417,8 +2427,13 @@
       <c r="Z54" s="4"/>
     </row>
     <row r="55" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="4"/>
-      <c r="B55" s="7"/>
+      <c r="A55" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="23">
+        <f>SUM(B3:B49)</f>
+        <v>113.18</v>
+      </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -2445,8 +2460,13 @@
       <c r="Z55" s="4"/>
     </row>
     <row r="56" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="4"/>
-      <c r="B56" s="7"/>
+      <c r="A56" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="23" t="e">
+        <f ca="1">MULTIPLY(B55,0.78)</f>
+        <v>#NAME?</v>
+      </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -29491,6 +29511,62 @@
       <c r="X1021" s="4"/>
       <c r="Y1021" s="4"/>
       <c r="Z1021" s="4"/>
+    </row>
+    <row r="1022" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1022" s="4"/>
+      <c r="B1022" s="7"/>
+      <c r="C1022" s="4"/>
+      <c r="D1022" s="4"/>
+      <c r="E1022" s="4"/>
+      <c r="F1022" s="4"/>
+      <c r="G1022" s="4"/>
+      <c r="H1022" s="4"/>
+      <c r="I1022" s="4"/>
+      <c r="J1022" s="4"/>
+      <c r="K1022" s="4"/>
+      <c r="L1022" s="4"/>
+      <c r="M1022" s="4"/>
+      <c r="N1022" s="4"/>
+      <c r="O1022" s="4"/>
+      <c r="P1022" s="4"/>
+      <c r="Q1022" s="4"/>
+      <c r="R1022" s="4"/>
+      <c r="S1022" s="4"/>
+      <c r="T1022" s="4"/>
+      <c r="U1022" s="4"/>
+      <c r="V1022" s="4"/>
+      <c r="W1022" s="4"/>
+      <c r="X1022" s="4"/>
+      <c r="Y1022" s="4"/>
+      <c r="Z1022" s="4"/>
+    </row>
+    <row r="1023" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1023" s="4"/>
+      <c r="B1023" s="7"/>
+      <c r="C1023" s="4"/>
+      <c r="D1023" s="4"/>
+      <c r="E1023" s="4"/>
+      <c r="F1023" s="4"/>
+      <c r="G1023" s="4"/>
+      <c r="H1023" s="4"/>
+      <c r="I1023" s="4"/>
+      <c r="J1023" s="4"/>
+      <c r="K1023" s="4"/>
+      <c r="L1023" s="4"/>
+      <c r="M1023" s="4"/>
+      <c r="N1023" s="4"/>
+      <c r="O1023" s="4"/>
+      <c r="P1023" s="4"/>
+      <c r="Q1023" s="4"/>
+      <c r="R1023" s="4"/>
+      <c r="S1023" s="4"/>
+      <c r="T1023" s="4"/>
+      <c r="U1023" s="4"/>
+      <c r="V1023" s="4"/>
+      <c r="W1023" s="4"/>
+      <c r="X1023" s="4"/>
+      <c r="Y1023" s="4"/>
+      <c r="Z1023" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -29526,6 +29602,8 @@
     <hyperlink ref="E51" r:id="rId30" display="https://www.amazon.com/Noctua-Cooling-Bearing-NF-A4X10-FLX-5V/dp/B00NEMGCIA" xr:uid="{8A7A47F3-F9B9-434F-8DF8-283F80FA298E}"/>
     <hyperlink ref="E3" r:id="rId31" display="https://www.amazon.com/MakerBeam-XL-Anodized-300x15x15mm-Pieces/dp/B06XJ4F9WW/ref=asc_df_B06XJ4F9WW?tag=bingshoppinga-20&amp;linkCode=df0&amp;hvadid=79852084166625&amp;hvnetw=o&amp;hvqmt=e&amp;hvbmt=be&amp;hvdev=c&amp;hvlocint=&amp;hvlocphy=&amp;hvtargid=pla-4583451672046415&amp;psc=1" xr:uid="{A5F373AC-C088-4C56-BBB1-B519B22139AD}"/>
     <hyperlink ref="E4" r:id="rId32" display="https://www.amazon.com/MakerBeam-XL-Anodized-50x15x15mm-100x15x15mm/dp/B06XJ4FZ12/ref=sr_1_20?adgrpid=1341404752136090&amp;dib=eyJ2IjoiMSJ9.l4Aa0aj5u6PwHLs6k2yd7X39huIxMysk6UVQpD-QmsnGjHj071QN20LucGBJIEps.iHlTyuyb18n7nTe47u5RaoZBfJQ9z6w4PqPGGdqF3ik&amp;dib_tag=se&amp;hvadid=83838037696959&amp;hvbmt=be&amp;hvdev=c&amp;hvlocphy=99357&amp;hvnetw=o&amp;hvqmt=e&amp;hvtargid=kwd-83838146055982%3Aloc-190&amp;hydadcr=8952_13537789&amp;keywords=makerbeam+xl+100mm&amp;msclkid=2b608a3375bc14e59940ec8528c4519f&amp;qid=1723227531&amp;sr=8-20" xr:uid="{EFD962DF-D345-4710-A1E4-61DF3488EF3F}"/>
+    <hyperlink ref="C52" r:id="rId33" display="https://www.aliexpress.us/item/3256805751725080.html?spm=a2g0o.order_list.order_list_main.22.5f9f1802hETnJh&amp;gatewayAdapt=glo2usa" xr:uid="{4C435BF2-6326-4A85-9279-3776C0044C57}"/>
+    <hyperlink ref="C53" r:id="rId34" display="https://www.aliexpress.us/item/3256804036608448.html?spm=a2g0o.order_list.order_list_main.81.6bd51802S5XSF7&amp;gatewayAdapt=glo2usa" xr:uid="{50126C93-7E4F-4F1F-B63C-767E3AFE1CDF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>